<commit_message>
build (v1.0.0): versión de resultados art. 1
</commit_message>
<xml_diff>
--- a/Repo/Articulo1/output/AHP.xlsx
+++ b/Repo/Articulo1/output/AHP.xlsx
@@ -9,10 +9,9 @@
   <sheets>
     <sheet name="info" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="alternative_info" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="alternatives" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="alternatives_norm" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="criteria" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="result" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="alternatives_norm" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="criteria" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="result" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -496,7 +495,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -711,10 +710,10 @@
         <v>500</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="D4" t="n">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -726,37 +725,37 @@
         <v>283.3442623937113</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>4.540635118306349</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>177.2139709590177</v>
+        <v>177.6305742311223</v>
       </c>
       <c r="K4" t="n">
-        <v>0.175</v>
+        <v>0.5625</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0008724607213740338</v>
+        <v>0.0008707763733645704</v>
       </c>
       <c r="M4" t="n">
-        <v>192.9064639749101</v>
+        <v>192.666453003929</v>
       </c>
       <c r="N4" t="n">
-        <v>15500</v>
+        <v>8362.5</v>
       </c>
       <c r="O4" t="n">
-        <v>21.75</v>
+        <v>22.5</v>
       </c>
       <c r="P4" t="n">
-        <v>0.57</v>
+        <v>0.4475</v>
       </c>
       <c r="Q4" t="n">
         <v>0</v>
       </c>
       <c r="R4" t="n">
-        <v>0.9166500000000001</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="5">
@@ -767,13 +766,13 @@
         <v>500</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="F5" t="n">
         <v>1918.506818181818</v>
@@ -782,37 +781,37 @@
         <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>4.540635118306349</v>
       </c>
       <c r="I5" t="n">
-        <v>5189.76</v>
+        <v>3113.856</v>
       </c>
       <c r="J5" t="n">
-        <v>1474.067744454545</v>
+        <v>941.1846101266499</v>
       </c>
       <c r="K5" t="n">
-        <v>65.81546400000002</v>
+        <v>39.9477784</v>
       </c>
       <c r="L5" t="n">
-        <v>0.8076223462626713</v>
+        <v>0.715368279423794</v>
       </c>
       <c r="M5" t="n">
-        <v>107.3404408132477</v>
+        <v>121.8776121123448</v>
       </c>
       <c r="N5" t="n">
-        <v>1550</v>
+        <v>1387.5</v>
       </c>
       <c r="O5" t="n">
-        <v>13.75</v>
+        <v>18.5</v>
       </c>
       <c r="P5" t="n">
-        <v>0.3</v>
+        <v>0.3125</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="R5" t="n">
-        <v>0.675</v>
+        <v>0.7541749999999999</v>
       </c>
     </row>
     <row r="6">
@@ -820,55 +819,55 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="C6" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>1918.506818181818</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>283.3442623937113</v>
       </c>
       <c r="H6" t="n">
-        <v>18.16254047322539</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>1.66641308841843</v>
+        <v>177.2139709590177</v>
       </c>
       <c r="K6" t="n">
-        <v>1.57</v>
+        <v>0.175</v>
       </c>
       <c r="L6" t="n">
-        <v>5.4e-05</v>
+        <v>0.0008724607213740338</v>
       </c>
       <c r="M6" t="n">
-        <v>76.28</v>
+        <v>192.9064639749101</v>
       </c>
       <c r="N6" t="n">
-        <v>1350</v>
+        <v>15500</v>
       </c>
       <c r="O6" t="n">
-        <v>40</v>
+        <v>21.75</v>
       </c>
       <c r="P6" t="n">
-        <v>0.4</v>
+        <v>0.57</v>
       </c>
       <c r="Q6" t="n">
         <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>0.6667</v>
+        <v>0.9166500000000001</v>
       </c>
     </row>
     <row r="7">
@@ -876,55 +875,55 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="C7" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>1918.506818181818</v>
       </c>
       <c r="G7" t="n">
         <v>283.3442623937113</v>
       </c>
       <c r="H7" t="n">
-        <v>9.081270236612697</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>3113.856</v>
       </c>
       <c r="J7" t="n">
-        <v>37.22877704868143</v>
+        <v>977.1635773590175</v>
       </c>
       <c r="K7" t="n">
-        <v>0.795</v>
+        <v>39.5602784</v>
       </c>
       <c r="L7" t="n">
-        <v>1.030057977833623e-05</v>
+        <v>0.686990975752078</v>
       </c>
       <c r="M7" t="n">
-        <v>123.4579328291089</v>
+        <v>122.0813954411684</v>
       </c>
       <c r="N7" t="n">
-        <v>15625</v>
+        <v>8525</v>
       </c>
       <c r="O7" t="n">
-        <v>38.5</v>
+        <v>17.75</v>
       </c>
       <c r="P7" t="n">
-        <v>0.645</v>
+        <v>0.435</v>
       </c>
       <c r="Q7" t="n">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="R7" t="n">
-        <v>0.75</v>
+        <v>0.795825</v>
       </c>
     </row>
     <row r="8">
@@ -932,10 +931,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="C8" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -944,43 +943,43 @@
         <v>500</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>1918.506818181818</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>9.081270236612697</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
         <v>5189.76</v>
       </c>
       <c r="J8" t="n">
-        <v>1334.082550544209</v>
+        <v>1474.067744454545</v>
       </c>
       <c r="K8" t="n">
-        <v>66.43546400000001</v>
+        <v>65.81546400000002</v>
       </c>
       <c r="L8" t="n">
-        <v>0.9988724023500071</v>
+        <v>0.8076223462626713</v>
       </c>
       <c r="M8" t="n">
-        <v>72.00747624991654</v>
+        <v>107.3404408132477</v>
       </c>
       <c r="N8" t="n">
-        <v>1675</v>
+        <v>1550</v>
       </c>
       <c r="O8" t="n">
-        <v>30.5</v>
+        <v>13.75</v>
       </c>
       <c r="P8" t="n">
-        <v>0.375</v>
+        <v>0.3</v>
       </c>
       <c r="Q8" t="n">
         <v>0.25</v>
       </c>
       <c r="R8" t="n">
-        <v>0.50835</v>
+        <v>0.675</v>
       </c>
     </row>
     <row r="9">
@@ -988,55 +987,55 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="D9" t="n">
-        <v>1000</v>
+        <v>250</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>959.2534090909091</v>
       </c>
       <c r="G9" t="n">
         <v>283.3442623937113</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>9.081270236612697</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>36.39557050447222</v>
+        <v>107.6379772759542</v>
       </c>
       <c r="K9" t="n">
-        <v>0.02</v>
+        <v>0.8725000000000001</v>
       </c>
       <c r="L9" t="n">
-        <v>8.899999999999999e-06</v>
+        <v>0.0007687798600300336</v>
       </c>
       <c r="M9" t="n">
-        <v>124.97</v>
+        <v>184.3708725246705</v>
       </c>
       <c r="N9" t="n">
-        <v>29900</v>
+        <v>8425</v>
       </c>
       <c r="O9" t="n">
-        <v>37</v>
+        <v>30.875</v>
       </c>
       <c r="P9" t="n">
-        <v>0.89</v>
+        <v>0.485</v>
       </c>
       <c r="Q9" t="n">
         <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>0.8333</v>
+        <v>0.7916749999999999</v>
       </c>
     </row>
     <row r="10">
@@ -1044,55 +1043,55 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="D10" t="n">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>959.2534090909091</v>
       </c>
       <c r="G10" t="n">
-        <v>283.3442623937113</v>
+        <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>9.081270236612697</v>
       </c>
       <c r="I10" t="n">
-        <v>5189.76</v>
+        <v>3113.856</v>
       </c>
       <c r="J10" t="n">
-        <v>1369.644914504472</v>
+        <v>871.1920131714818</v>
       </c>
       <c r="K10" t="n">
-        <v>65.66046400000002</v>
+        <v>40.2577784</v>
       </c>
       <c r="L10" t="n">
-        <v>0.9659750604142714</v>
+        <v>0.8330618797555602</v>
       </c>
       <c r="M10" t="n">
-        <v>74.74227291486508</v>
+        <v>102.7784518394114</v>
       </c>
       <c r="N10" t="n">
-        <v>15950</v>
+        <v>1450</v>
       </c>
       <c r="O10" t="n">
-        <v>29</v>
+        <v>26.875</v>
       </c>
       <c r="P10" t="n">
-        <v>0.62</v>
+        <v>0.35</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="R10" t="n">
-        <v>0.5916500000000001</v>
+        <v>0.6708499999999999</v>
       </c>
     </row>
     <row r="11">
@@ -1100,54 +1099,782 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>959.2534090909091</v>
+      </c>
+      <c r="G11" t="n">
+        <v>283.3442623937113</v>
+      </c>
+      <c r="H11" t="n">
+        <v>4.540635118306349</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>107.2213740038495</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.485</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.000771382261477513</v>
+      </c>
+      <c r="M11" t="n">
+        <v>184.7644144511396</v>
+      </c>
+      <c r="N11" t="n">
+        <v>15562.5</v>
+      </c>
+      <c r="O11" t="n">
+        <v>30.125</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.6075</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.8333250000000001</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>250</v>
+      </c>
+      <c r="C12" t="n">
+        <v>250</v>
+      </c>
+      <c r="D12" t="n">
+        <v>250</v>
+      </c>
+      <c r="E12" t="n">
+        <v>250</v>
+      </c>
+      <c r="F12" t="n">
+        <v>959.2534090909091</v>
+      </c>
+      <c r="G12" t="n">
+        <v>283.3442623937113</v>
+      </c>
+      <c r="H12" t="n">
+        <v>4.540635118306349</v>
+      </c>
+      <c r="I12" t="n">
+        <v>3113.856</v>
+      </c>
+      <c r="J12" t="n">
+        <v>907.1709804038494</v>
+      </c>
+      <c r="K12" t="n">
+        <v>39.8702784</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.7948213272716566</v>
+      </c>
+      <c r="M12" t="n">
+        <v>104.247879954976</v>
+      </c>
+      <c r="N12" t="n">
+        <v>8587.5</v>
+      </c>
+      <c r="O12" t="n">
+        <v>26.125</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.4725</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.7125</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>250</v>
+      </c>
+      <c r="C13" t="n">
+        <v>250</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>500</v>
+      </c>
+      <c r="F13" t="n">
+        <v>959.2534090909091</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>4.540635118306349</v>
+      </c>
+      <c r="I13" t="n">
+        <v>5189.76</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1404.075147499377</v>
+      </c>
+      <c r="K13" t="n">
+        <v>66.12546400000001</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.8931124691265738</v>
+      </c>
+      <c r="M13" t="n">
+        <v>92.41488128683751</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1612.5</v>
+      </c>
+      <c r="O13" t="n">
+        <v>22.125</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.3375</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.591675</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>250</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>500</v>
+      </c>
+      <c r="E14" t="n">
+        <v>250</v>
+      </c>
+      <c r="F14" t="n">
+        <v>959.2534090909091</v>
+      </c>
+      <c r="G14" t="n">
+        <v>283.3442623937113</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>3113.856</v>
+      </c>
+      <c r="J14" t="n">
+        <v>906.7543771317448</v>
+      </c>
+      <c r="K14" t="n">
+        <v>39.4827784</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.7954159399187822</v>
+      </c>
+      <c r="M14" t="n">
+        <v>104.2770302564561</v>
+      </c>
+      <c r="N14" t="n">
+        <v>15725</v>
+      </c>
+      <c r="O14" t="n">
+        <v>25.375</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.595</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.7541500000000001</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>250</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>250</v>
+      </c>
+      <c r="E15" t="n">
+        <v>500</v>
+      </c>
+      <c r="F15" t="n">
+        <v>959.2534090909091</v>
+      </c>
+      <c r="G15" t="n">
+        <v>283.3442623937113</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>5189.76</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1440.054114731745</v>
+      </c>
+      <c r="K15" t="n">
+        <v>65.73796400000002</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.8662999274196177</v>
+      </c>
+      <c r="M15" t="n">
+        <v>93.8603184317181</v>
+      </c>
+      <c r="N15" t="n">
+        <v>8750</v>
+      </c>
+      <c r="O15" t="n">
+        <v>21.375</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.633325</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
         <v>1000</v>
       </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>18.16254047322539</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1.66641308841843</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="L16" t="n">
+        <v>5.4e-05</v>
+      </c>
+      <c r="M16" t="n">
+        <v>76.28</v>
+      </c>
+      <c r="N16" t="n">
+        <v>1350</v>
+      </c>
+      <c r="O16" t="n">
+        <v>40</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.6667</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>500</v>
+      </c>
+      <c r="D17" t="n">
+        <v>500</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>283.3442623937113</v>
+      </c>
+      <c r="H17" t="n">
+        <v>9.081270236612697</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>37.22877704868143</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.795</v>
+      </c>
+      <c r="L17" t="n">
+        <v>1.030057977833623e-05</v>
+      </c>
+      <c r="M17" t="n">
+        <v>123.4579328291089</v>
+      </c>
+      <c r="N17" t="n">
+        <v>15625</v>
+      </c>
+      <c r="O17" t="n">
+        <v>38.5</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.645</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>500</v>
+      </c>
+      <c r="D18" t="n">
+        <v>250</v>
+      </c>
+      <c r="E18" t="n">
+        <v>250</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>283.3442623937113</v>
+      </c>
+      <c r="H18" t="n">
+        <v>9.081270236612697</v>
+      </c>
+      <c r="I18" t="n">
+        <v>3113.856</v>
+      </c>
+      <c r="J18" t="n">
+        <v>837.1783834486813</v>
+      </c>
+      <c r="K18" t="n">
+        <v>40.1802784</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.9428739793268266</v>
+      </c>
+      <c r="M18" t="n">
+        <v>76.41760708017222</v>
+      </c>
+      <c r="N18" t="n">
+        <v>8650</v>
+      </c>
+      <c r="O18" t="n">
+        <v>34.5</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.6291749999999999</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>500</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>500</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="n">
+        <v>9.081270236612697</v>
+      </c>
+      <c r="I19" t="n">
+        <v>5189.76</v>
+      </c>
+      <c r="J19" t="n">
+        <v>1334.082550544209</v>
+      </c>
+      <c r="K19" t="n">
+        <v>66.43546400000001</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.9988724023500071</v>
+      </c>
+      <c r="M19" t="n">
+        <v>72.00747624991654</v>
+      </c>
+      <c r="N19" t="n">
+        <v>1675</v>
+      </c>
+      <c r="O19" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.50835</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>250</v>
+      </c>
+      <c r="D20" t="n">
+        <v>500</v>
+      </c>
+      <c r="E20" t="n">
+        <v>250</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>283.3442623937113</v>
+      </c>
+      <c r="H20" t="n">
+        <v>4.540635118306349</v>
+      </c>
+      <c r="I20" t="n">
+        <v>3113.856</v>
+      </c>
+      <c r="J20" t="n">
+        <v>836.7617801765767</v>
+      </c>
+      <c r="K20" t="n">
+        <v>39.7927784</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.9437110342246948</v>
+      </c>
+      <c r="M20" t="n">
+        <v>76.41779075775368</v>
+      </c>
+      <c r="N20" t="n">
+        <v>15787.5</v>
+      </c>
+      <c r="O20" t="n">
+        <v>33.75</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.6325</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.670825</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>250</v>
+      </c>
+      <c r="D21" t="n">
+        <v>250</v>
+      </c>
+      <c r="E21" t="n">
+        <v>500</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>283.3442623937113</v>
+      </c>
+      <c r="H21" t="n">
+        <v>4.540635118306349</v>
+      </c>
+      <c r="I21" t="n">
+        <v>5189.76</v>
+      </c>
+      <c r="J21" t="n">
+        <v>1370.061517776577</v>
+      </c>
+      <c r="K21" t="n">
+        <v>66.04796400000001</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.9654486695958249</v>
+      </c>
+      <c r="M21" t="n">
+        <v>74.74354759727619</v>
+      </c>
+      <c r="N21" t="n">
+        <v>8812.5</v>
+      </c>
+      <c r="O21" t="n">
+        <v>29.75</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.4975</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.55</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>283.3442623937113</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>36.39557050447222</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="L22" t="n">
+        <v>8.899999999999999e-06</v>
+      </c>
+      <c r="M22" t="n">
+        <v>124.97</v>
+      </c>
+      <c r="N22" t="n">
+        <v>29900</v>
+      </c>
+      <c r="O22" t="n">
+        <v>37</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0.8333</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>500</v>
+      </c>
+      <c r="E23" t="n">
+        <v>500</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>283.3442623937113</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
+        <v>5189.76</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1369.644914504472</v>
+      </c>
+      <c r="K23" t="n">
+        <v>65.66046400000002</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.9659750604142714</v>
+      </c>
+      <c r="M23" t="n">
+        <v>74.74227291486508</v>
+      </c>
+      <c r="N23" t="n">
+        <v>15950</v>
+      </c>
+      <c r="O23" t="n">
+        <v>29</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0.5916500000000001</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
         <v>6701.532</v>
       </c>
-      <c r="J11" t="n">
+      <c r="J24" t="n">
         <v>1721.6235708</v>
       </c>
-      <c r="K11" t="n">
+      <c r="K24" t="n">
         <v>84.77437980000001</v>
       </c>
-      <c r="L11" t="n">
+      <c r="L24" t="n">
         <v>1</v>
       </c>
-      <c r="M11" t="n">
+      <c r="M24" t="n">
         <v>72</v>
       </c>
-      <c r="N11" t="n">
+      <c r="N24" t="n">
         <v>2000</v>
       </c>
-      <c r="O11" t="n">
+      <c r="O24" t="n">
         <v>21</v>
       </c>
-      <c r="P11" t="n">
+      <c r="P24" t="n">
         <v>0.35</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="Q24" t="n">
         <v>0.5</v>
       </c>
-      <c r="R11" t="n">
+      <c r="R24" t="n">
         <v>0.35</v>
       </c>
     </row>
@@ -1162,7 +1889,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1222,31 +1949,31 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.04283311387432179</v>
+        <v>0.01613104921568008</v>
       </c>
       <c r="C2" t="n">
-        <v>0.04907429220286972</v>
+        <v>0.04525804779853988</v>
       </c>
       <c r="D2" t="n">
-        <v>0.004326851808698382</v>
+        <v>0.004257629970652742</v>
       </c>
       <c r="E2" t="n">
-        <v>0.05201322853100841</v>
+        <v>0.02269748542388596</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2050739228983865</v>
+        <v>0.1216971652958431</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3025781706405269</v>
+        <v>0.1496591726945724</v>
       </c>
       <c r="H2" t="n">
-        <v>0.05291005291005291</v>
+        <v>0.02300437083045779</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1403508771929824</v>
+        <v>0.06102212051868802</v>
       </c>
     </row>
     <row r="3">
@@ -1254,31 +1981,31 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.02154327628162776</v>
+        <v>0.008113247404463496</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01704685939678632</v>
+        <v>0.01572121660370333</v>
       </c>
       <c r="D3" t="n">
-        <v>0.004346222067106116</v>
+        <v>0.004276690339803879</v>
       </c>
       <c r="E3" t="n">
-        <v>0.05216661847155036</v>
+        <v>0.02276442158681893</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1841480123985511</v>
+        <v>0.1092790872044305</v>
       </c>
       <c r="G3" t="n">
-        <v>0.08459174663068494</v>
+        <v>0.04184019881783742</v>
       </c>
       <c r="H3" t="n">
-        <v>0.06878306878306878</v>
+        <v>0.02990568207959513</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1169614035087719</v>
+        <v>0.05085278413424865</v>
       </c>
     </row>
     <row r="4">
@@ -1286,31 +2013,31 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.02695182651452757</v>
+        <v>0.01017398126197526</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0925400938682686</v>
+        <v>0.02655138804181006</v>
       </c>
       <c r="D4" t="n">
-        <v>0.004959365737272442</v>
+        <v>0.00488946427680599</v>
       </c>
       <c r="E4" t="n">
-        <v>0.05471856349746645</v>
+        <v>0.02390778269961446</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01455363323795001</v>
+        <v>0.01600799782665798</v>
       </c>
       <c r="G4" t="n">
-        <v>0.09042566019142186</v>
+        <v>0.04323487211176534</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1206349206349206</v>
+        <v>0.04117782378651944</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1286526315789474</v>
+        <v>0.05339435545385201</v>
       </c>
     </row>
     <row r="5">
@@ -1318,31 +2045,31 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2241855870854985</v>
+        <v>0.05390735592077089</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0002460594432175849</v>
+        <v>0.0003738669926515403</v>
       </c>
       <c r="D5" t="n">
-        <v>5.357518682737285e-06</v>
+        <v>5.951661672896826e-06</v>
       </c>
       <c r="E5" t="n">
-        <v>0.09833725777638229</v>
+        <v>0.03779387872874857</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1455363323795001</v>
+        <v>0.09648063554985757</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1430369533937036</v>
+        <v>0.05258295256836326</v>
       </c>
       <c r="H5" t="n">
-        <v>0.06349206349206349</v>
+        <v>0.02875546353807223</v>
       </c>
       <c r="I5" t="n">
-        <v>0.2</v>
+        <v>0.04347826086956522</v>
       </c>
       <c r="J5" t="n">
-        <v>0.09473684210526316</v>
+        <v>0.04602135774218153</v>
       </c>
     </row>
     <row r="6">
@@ -1350,31 +2077,31 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0002534386889337191</v>
+        <v>0.01015011986366353</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01031497861588981</v>
+        <v>0.08534374727724663</v>
       </c>
       <c r="D6" t="n">
-        <v>0.08012688534626633</v>
+        <v>0.004880024815268958</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1383791898018202</v>
+        <v>0.02387803703935247</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1670972705097964</v>
+        <v>0.008636573020995315</v>
       </c>
       <c r="G6" t="n">
-        <v>0.04916895272908563</v>
+        <v>0.04472572977079173</v>
       </c>
       <c r="H6" t="n">
-        <v>0.08465608465608467</v>
+        <v>0.05244996549344375</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0935719298245614</v>
+        <v>0.05593592677345537</v>
       </c>
     </row>
     <row r="7">
@@ -1382,31 +2109,31 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.005661988921833534</v>
+        <v>0.05596808977828265</v>
       </c>
       <c r="C7" t="n">
-        <v>0.02037046091439875</v>
+        <v>0.0003775290866890907</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4200590551027473</v>
+        <v>6.19750494683243e-06</v>
       </c>
       <c r="E7" t="n">
-        <v>0.08549928187031866</v>
+        <v>0.03773079161880303</v>
       </c>
       <c r="F7" t="n">
-        <v>0.01443720417204641</v>
+        <v>0.0157028600381733</v>
       </c>
       <c r="G7" t="n">
-        <v>0.05108462621203702</v>
+        <v>0.05480476746561804</v>
       </c>
       <c r="H7" t="n">
-        <v>0.1365079365079365</v>
+        <v>0.04002760524499655</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>0.04347826086956522</v>
       </c>
       <c r="J7" t="n">
-        <v>0.1052631578947368</v>
+        <v>0.04856292906178489</v>
       </c>
     </row>
     <row r="8">
@@ -1414,31 +2141,31 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.2028957494928045</v>
+        <v>0.08442880779887192</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0002437631266780496</v>
+        <v>0.0002269247205112488</v>
       </c>
       <c r="D8" t="n">
-        <v>4.33173626433043e-06</v>
+        <v>5.271808030517261e-06</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1465898424414657</v>
+        <v>0.04291232323088175</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1346754120526717</v>
+        <v>0.08636573020995315</v>
       </c>
       <c r="G8" t="n">
-        <v>0.06448387243158771</v>
+        <v>0.07074797254652511</v>
       </c>
       <c r="H8" t="n">
-        <v>0.07936507936507936</v>
+        <v>0.02760524499654935</v>
       </c>
       <c r="I8" t="n">
-        <v>0.2</v>
+        <v>0.08695652173913043</v>
       </c>
       <c r="J8" t="n">
-        <v>0.07134736842105263</v>
+        <v>0.04118993135011441</v>
       </c>
     </row>
     <row r="9">
@@ -1446,31 +2173,31 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.005535269577366674</v>
+        <v>0.006165080356366966</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8097258213473503</v>
+        <v>0.01711765704701222</v>
       </c>
       <c r="D9" t="n">
-        <v>0.4861631245728519</v>
+        <v>0.005538165334464421</v>
       </c>
       <c r="E9" t="n">
-        <v>0.08446478833386291</v>
+        <v>0.02498348914255456</v>
       </c>
       <c r="F9" t="n">
-        <v>0.007544525591579435</v>
+        <v>0.01588924413358189</v>
       </c>
       <c r="G9" t="n">
-        <v>0.05315562457198447</v>
+        <v>0.03150719425148892</v>
       </c>
       <c r="H9" t="n">
-        <v>0.1883597883597884</v>
+        <v>0.04462847941108811</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>0.1169543859649123</v>
+        <v>0.04830968726163233</v>
       </c>
     </row>
     <row r="10">
@@ -1478,31 +2205,31 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.2083042997257043</v>
+        <v>0.0498984550151626</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0002466402982919372</v>
+        <v>0.0003709880765183546</v>
       </c>
       <c r="D10" t="n">
-        <v>4.479258301806211e-06</v>
+        <v>5.110820785488384e-06</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1412261654138632</v>
+        <v>0.04481705658614633</v>
       </c>
       <c r="F10" t="n">
-        <v>0.01414302916540596</v>
+        <v>0.09232198746581198</v>
       </c>
       <c r="G10" t="n">
-        <v>0.06781924514356638</v>
+        <v>0.0361966371168268</v>
       </c>
       <c r="H10" t="n">
-        <v>0.1312169312169312</v>
+        <v>0.0322061191626409</v>
       </c>
       <c r="I10" t="n">
-        <v>0.2</v>
+        <v>0.04347826086956522</v>
       </c>
       <c r="J10" t="n">
-        <v>0.08303859649122809</v>
+        <v>0.04093668954996185</v>
       </c>
     </row>
     <row r="11">
@@ -1510,31 +2237,447 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.2618354498373816</v>
+        <v>0.006141218958055237</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0001910307862487837</v>
+        <v>0.03079413561550136</v>
       </c>
       <c r="D11" t="n">
-        <v>4.326851808698382e-06</v>
+        <v>0.005519481304246791</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1466050638622618</v>
+        <v>0.02493027515935175</v>
       </c>
       <c r="F11" t="n">
-        <v>0.1127906575941126</v>
+        <v>0.008601887988782482</v>
       </c>
       <c r="G11" t="n">
-        <v>0.09365514805540121</v>
+        <v>0.03229160572662972</v>
       </c>
       <c r="H11" t="n">
-        <v>0.07407407407407407</v>
+        <v>0.05590062111801243</v>
       </c>
       <c r="I11" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>0.04912280701754386</v>
+        <v>0.05085125858123569</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.05195918887267436</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0003745937167451071</v>
+      </c>
+      <c r="D12" t="n">
+        <v>5.356713294631505e-06</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.04418533685205702</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.01558857430281542</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0372357750244869</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.04347826086956522</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.04347826086956522</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.04347826086956521</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.08041990689326363</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.0002258608842959221</v>
+      </c>
+      <c r="D13" t="n">
+        <v>4.767182317828934e-06</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.04984292170031142</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.08301822128708675</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.04396766655433764</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.03105590062111802</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.08695652173913043</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.03610526315789473</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.05193532747436263</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.000378270131402864</v>
+      </c>
+      <c r="D14" t="n">
+        <v>5.352708887236377e-06</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.04417298498619478</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.008512997254399197</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.03833633980353578</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.05475040257648953</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.04347826086956522</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.04601983218916857</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.08248064075077539</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0002271922472913544</v>
+      </c>
+      <c r="D15" t="n">
+        <v>4.914729686443151e-06</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.049075346950526</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.01529907220862027</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.0455103916965951</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.04232804232804233</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.08695652173913043</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.03864683447749809</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>9.544559324691378e-05</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.009512838072304559</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.07884499945653226</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.0603857851589331</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.09916065320402027</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.024319615562868</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.03680699332873247</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.0406834477498093</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.002132318052446946</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.01878635946354485</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.4133388665759593</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.03731009896544584</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.008567480436827353</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.02526713305233039</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.0593512767425811</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.04576659038901601</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.04795028796706607</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0003717036408965787</v>
+      </c>
+      <c r="D18" t="n">
+        <v>4.515587516470138e-06</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.06027704697807237</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.01547594009542513</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.02819665572506435</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.04692891649413389</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.04347826086956522</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.03839359267734552</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.07641100598765535</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.000224806976188473</v>
+      </c>
+      <c r="D19" t="n">
+        <v>4.262436283789588e-06</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.06396874230026574</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.07992052646294172</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.03189457778736787</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.03450655624568668</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.08695652173913043</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.03102059496567505</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.04792642656875435</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0003753232715591972</v>
+      </c>
+      <c r="D20" t="n">
+        <v>4.511582270679494e-06</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.06027690209633611</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.008479295760913849</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.02882324807451023</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.0582010582010582</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.04347826086956522</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.04093516399694889</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.07847173984516712</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0002261259071289186</v>
+      </c>
+      <c r="D21" t="n">
+        <v>4.410001385609817e-06</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.06162709477936631</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.01519056815040311</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.03269864277360404</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.045778697952611</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.08695652173913043</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.03356216628527841</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.002084595255823489</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.746757788675908</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.4783853899609822</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.03685866761561508</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.004477153238308608</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.02629147628418163</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.08189556015642974</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.05084973302822272</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.07844787844685537</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0002274604056029539</v>
+      </c>
+      <c r="D23" t="n">
+        <v>4.407598234292715e-06</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.06162814579067088</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.008392907951437453</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.0335442973280938</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.05705083965953532</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.08695652173913043</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.03610373760488177</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.09860783271861556</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0001761753469474295</v>
+      </c>
+      <c r="D24" t="n">
+        <v>4.257629970652742e-06</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.06397538461004745</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.06693344091271369</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.04632307726260573</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.0322061191626409</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.1739130434782609</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.0213577421815408</v>
       </c>
     </row>
   </sheetData>
@@ -1543,392 +2686,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>C1.1</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>C1.2</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>C1.4</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>C2.1</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>C2.2</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>C2.3</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>C3.1</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>C3.2</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>C3.3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.04283311387432179</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.04907429220286972</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.004326851808698382</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.05201322853100841</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.2050739228983865</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.3025781706405269</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.05291005291005291</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.1403508771929824</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>0.02154327628162776</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.01704685939678632</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.004346222067106116</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.05216661847155036</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.1841480123985511</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.08459174663068494</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.06878306878306878</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.1169614035087719</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0.02695182651452757</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0925400938682686</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.004959365737272442</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.05471856349746645</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.01455363323795001</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.09042566019142186</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.1206349206349206</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.1286526315789474</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0.2241855870854985</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.0002460594432175849</v>
-      </c>
-      <c r="D5" t="n">
-        <v>5.357518682737285e-06</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.09833725777638229</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.1455363323795001</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.1430369533937036</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.06349206349206349</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.09473684210526316</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0.0002534386889337191</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.01031497861588981</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.08012688534626633</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.1383791898018202</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.1670972705097964</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.04916895272908563</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.08465608465608467</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.0935719298245614</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0.005661988921833534</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.02037046091439875</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.4200590551027473</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.08549928187031866</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.01443720417204641</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.05108462621203702</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.1365079365079365</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.1052631578947368</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0.2028957494928045</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.0002437631266780496</v>
-      </c>
-      <c r="D8" t="n">
-        <v>4.33173626433043e-06</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.1465898424414657</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.1346754120526717</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.06448387243158771</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.07936507936507936</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.07134736842105263</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.005535269577366674</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.8097258213473503</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.4861631245728519</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.08446478833386291</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.007544525591579435</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.05315562457198447</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.1883597883597884</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.1169543859649123</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.2083042997257043</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.0002466402982919372</v>
-      </c>
-      <c r="D10" t="n">
-        <v>4.479258301806211e-06</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.1412261654138632</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.01414302916540596</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.06781924514356638</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.1312169312169312</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.08303859649122809</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.2618354498373816</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.0001910307862487837</v>
-      </c>
-      <c r="D11" t="n">
-        <v>4.326851808698382e-06</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.1466050638622618</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.1127906575941126</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.09365514805540121</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.07407407407407407</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.04912280701754386</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2024,13 +2781,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2047,82 +2804,186 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1946559253688551</v>
+        <v>0.1586222626906079</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1264753953420925</v>
+        <v>0.06783556929757241</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1077307170215902</v>
+        <v>0.05594411925592701</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>0.09995615767417822</v>
+        <v>0.04930300463870221</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>0.09435116778431633</v>
+        <v>0.04893763648895198</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B7" t="n">
-        <v>0.09399993185703255</v>
+        <v>0.04573300333552847</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B8" t="n">
-        <v>0.09320930128845055</v>
+        <v>0.04498973276679945</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B9" t="n">
-        <v>0.06928541446360424</v>
+        <v>0.04026179961382692</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B10" t="n">
-        <v>0.06106524528201637</v>
+        <v>0.0400587730142406</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.03993330261909819</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.03939066304823054</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.03886775312516076</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.0378034782959355</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.03296211451876218</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.0320555767135463</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.03195441866600065</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.03177779156157975</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.03141703646343348</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.03123076889278729</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.03108706756564101</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B11" t="n">
-        <v>0.05927074391786388</v>
+      <c r="B22" t="n">
+        <v>0.02437085171766673</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.02389227605020171</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.02157099965979882</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test (art 1): resultados articulo 1 versión inicial
</commit_message>
<xml_diff>
--- a/Repo/Articulo1/output/AHP.xlsx
+++ b/Repo/Articulo1/output/AHP.xlsx
@@ -480,7 +480,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1 // 0 - expertos; 1 - Igual importancia; 2 - Enfoque Ambiental; 3 - Enfoque Económico; 4 - Enfoque Técnico</t>
+          <t xml:space="preserve"> 0 // 0 - expertos; 1 - Igual importancia; 2 - Enfoque Ambiental; 3 - Enfoque Económico; 4 - Enfoque Técnico</t>
         </is>
       </c>
     </row>
@@ -722,7 +722,7 @@
         <v>1918.506818181818</v>
       </c>
       <c r="G4" t="n">
-        <v>283.3442623937113</v>
+        <v>640.793947259624</v>
       </c>
       <c r="H4" t="n">
         <v>4.540635118306349</v>
@@ -731,16 +731,16 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>177.6305742311223</v>
+        <v>223.5449862521488</v>
       </c>
       <c r="K4" t="n">
         <v>0.5625</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0008707763733645704</v>
+        <v>0.0007506139335251635</v>
       </c>
       <c r="M4" t="n">
-        <v>192.666453003929</v>
+        <v>183.2282421272689</v>
       </c>
       <c r="N4" t="n">
         <v>8362.5</v>
@@ -834,7 +834,7 @@
         <v>1918.506818181818</v>
       </c>
       <c r="G6" t="n">
-        <v>283.3442623937113</v>
+        <v>1067.989912099374</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -843,16 +843,16 @@
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>177.2139709590177</v>
+        <v>278.00170466371</v>
       </c>
       <c r="K6" t="n">
         <v>0.175</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0008724607213740338</v>
+        <v>0.0006455764403994414</v>
       </c>
       <c r="M6" t="n">
-        <v>192.9064639749101</v>
+        <v>175.0574402764045</v>
       </c>
       <c r="N6" t="n">
         <v>15500</v>
@@ -890,7 +890,7 @@
         <v>1918.506818181818</v>
       </c>
       <c r="G7" t="n">
-        <v>283.3442623937113</v>
+        <v>640.793947259624</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -899,16 +899,16 @@
         <v>3113.856</v>
       </c>
       <c r="J7" t="n">
-        <v>977.1635773590175</v>
+        <v>1023.077989380044</v>
       </c>
       <c r="K7" t="n">
         <v>39.5602784</v>
       </c>
       <c r="L7" t="n">
-        <v>0.686990975752078</v>
+        <v>0.6537430848820482</v>
       </c>
       <c r="M7" t="n">
-        <v>122.0813954411684</v>
+        <v>122.2633983069356</v>
       </c>
       <c r="N7" t="n">
         <v>8525</v>
@@ -1002,7 +1002,7 @@
         <v>959.2534090909091</v>
       </c>
       <c r="G9" t="n">
-        <v>283.3442623937113</v>
+        <v>640.793947259624</v>
       </c>
       <c r="H9" t="n">
         <v>9.081270236612697</v>
@@ -1011,16 +1011,16 @@
         <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>107.6379772759542</v>
+        <v>153.5523892969807</v>
       </c>
       <c r="K9" t="n">
         <v>0.8725000000000001</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0007687798600300336</v>
+        <v>0.0005999811623896996</v>
       </c>
       <c r="M9" t="n">
-        <v>184.3708725246705</v>
+        <v>171.1756420043254</v>
       </c>
       <c r="N9" t="n">
         <v>8425</v>
@@ -1114,7 +1114,7 @@
         <v>959.2534090909091</v>
       </c>
       <c r="G11" t="n">
-        <v>283.3442623937113</v>
+        <v>1067.989912099374</v>
       </c>
       <c r="H11" t="n">
         <v>4.540635118306349</v>
@@ -1123,16 +1123,16 @@
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>107.2213740038495</v>
+        <v>208.0091077085419</v>
       </c>
       <c r="K11" t="n">
         <v>0.485</v>
       </c>
       <c r="L11" t="n">
-        <v>0.000771382261477513</v>
+        <v>0.0004769226130545392</v>
       </c>
       <c r="M11" t="n">
-        <v>184.7644144511396</v>
+        <v>161.6726742933793</v>
       </c>
       <c r="N11" t="n">
         <v>15562.5</v>
@@ -1170,7 +1170,7 @@
         <v>959.2534090909091</v>
       </c>
       <c r="G12" t="n">
-        <v>283.3442623937113</v>
+        <v>640.793947259624</v>
       </c>
       <c r="H12" t="n">
         <v>4.540635118306349</v>
@@ -1179,16 +1179,16 @@
         <v>3113.856</v>
       </c>
       <c r="J12" t="n">
-        <v>907.1709804038494</v>
+        <v>953.0853924248759</v>
       </c>
       <c r="K12" t="n">
         <v>39.8702784</v>
       </c>
       <c r="L12" t="n">
-        <v>0.7948213272716566</v>
+        <v>0.7506442802556406</v>
       </c>
       <c r="M12" t="n">
-        <v>104.247879954976</v>
+        <v>105.8177015515107</v>
       </c>
       <c r="N12" t="n">
         <v>8587.5</v>
@@ -1282,7 +1282,7 @@
         <v>959.2534090909091</v>
       </c>
       <c r="G14" t="n">
-        <v>283.3442623937113</v>
+        <v>1067.989912099374</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1291,16 +1291,16 @@
         <v>3113.856</v>
       </c>
       <c r="J14" t="n">
-        <v>906.7543771317448</v>
+        <v>1007.542110836437</v>
       </c>
       <c r="K14" t="n">
         <v>39.4827784</v>
       </c>
       <c r="L14" t="n">
-        <v>0.7954159399187822</v>
+        <v>0.7043540549013443</v>
       </c>
       <c r="M14" t="n">
-        <v>104.2770302564561</v>
+        <v>107.4352358608177</v>
       </c>
       <c r="N14" t="n">
         <v>15725</v>
@@ -1338,7 +1338,7 @@
         <v>959.2534090909091</v>
       </c>
       <c r="G15" t="n">
-        <v>283.3442623937113</v>
+        <v>640.793947259624</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1347,16 +1347,16 @@
         <v>5189.76</v>
       </c>
       <c r="J15" t="n">
-        <v>1440.054114731745</v>
+        <v>1485.968526752771</v>
       </c>
       <c r="K15" t="n">
         <v>65.73796400000002</v>
       </c>
       <c r="L15" t="n">
-        <v>0.8662999274196177</v>
+        <v>0.8341918991733863</v>
       </c>
       <c r="M15" t="n">
-        <v>93.8603184317181</v>
+        <v>95.49808888516999</v>
       </c>
       <c r="N15" t="n">
         <v>8750</v>
@@ -1450,7 +1450,7 @@
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>283.3442623937113</v>
+        <v>1067.989912099374</v>
       </c>
       <c r="H17" t="n">
         <v>9.081270236612697</v>
@@ -1459,16 +1459,16 @@
         <v>0</v>
       </c>
       <c r="J17" t="n">
-        <v>37.22877704868143</v>
+        <v>138.0165107533738</v>
       </c>
       <c r="K17" t="n">
         <v>0.795</v>
       </c>
       <c r="L17" t="n">
-        <v>1.030057977833623e-05</v>
+        <v>9.280258328686273e-06</v>
       </c>
       <c r="M17" t="n">
-        <v>123.4579328291089</v>
+        <v>124.5594727710923</v>
       </c>
       <c r="N17" t="n">
         <v>15625</v>
@@ -1506,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>283.3442623937113</v>
+        <v>640.793947259624</v>
       </c>
       <c r="H18" t="n">
         <v>9.081270236612697</v>
@@ -1515,16 +1515,16 @@
         <v>3113.856</v>
       </c>
       <c r="J18" t="n">
-        <v>837.1783834486813</v>
+        <v>883.0927954697078</v>
       </c>
       <c r="K18" t="n">
         <v>40.1802784</v>
       </c>
       <c r="L18" t="n">
-        <v>0.9428739793268266</v>
+        <v>0.8813317657511304</v>
       </c>
       <c r="M18" t="n">
-        <v>76.41760708017222</v>
+        <v>81.02873272804024</v>
       </c>
       <c r="N18" t="n">
         <v>8650</v>
@@ -1618,7 +1618,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>283.3442623937113</v>
+        <v>1067.989912099374</v>
       </c>
       <c r="H20" t="n">
         <v>4.540635118306349</v>
@@ -1627,16 +1627,16 @@
         <v>3113.856</v>
       </c>
       <c r="J20" t="n">
-        <v>836.7617801765767</v>
+        <v>937.549513881269</v>
       </c>
       <c r="K20" t="n">
         <v>39.7927784</v>
       </c>
       <c r="L20" t="n">
-        <v>0.9437110342246948</v>
+        <v>0.8181862245994608</v>
       </c>
       <c r="M20" t="n">
-        <v>76.41779075775368</v>
+        <v>85.51782949900341</v>
       </c>
       <c r="N20" t="n">
         <v>15787.5</v>
@@ -1674,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>283.3442623937113</v>
+        <v>640.793947259624</v>
       </c>
       <c r="H21" t="n">
         <v>4.540635118306349</v>
@@ -1683,16 +1683,16 @@
         <v>5189.76</v>
       </c>
       <c r="J21" t="n">
-        <v>1370.061517776577</v>
+        <v>1415.975929797603</v>
       </c>
       <c r="K21" t="n">
         <v>66.04796400000001</v>
       </c>
       <c r="L21" t="n">
-        <v>0.9654486695958249</v>
+        <v>0.9257343445581757</v>
       </c>
       <c r="M21" t="n">
-        <v>74.74354759727619</v>
+        <v>77.82034940911073</v>
       </c>
       <c r="N21" t="n">
         <v>8812.5</v>
@@ -1730,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>283.3442623937113</v>
+        <v>2135.979824198747</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -1739,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>36.39557050447222</v>
+        <v>274.3666084183291</v>
       </c>
       <c r="K22" t="n">
         <v>0.02</v>
@@ -1786,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>283.3442623937113</v>
+        <v>1067.989912099374</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -1795,16 +1795,16 @@
         <v>5189.76</v>
       </c>
       <c r="J23" t="n">
-        <v>1369.644914504472</v>
+        <v>1470.432648209164</v>
       </c>
       <c r="K23" t="n">
         <v>65.66046400000002</v>
       </c>
       <c r="L23" t="n">
-        <v>0.9659750604142714</v>
+        <v>0.8827955896432095</v>
       </c>
       <c r="M23" t="n">
-        <v>74.74227291486508</v>
+        <v>81.04021835940149</v>
       </c>
       <c r="N23" t="n">
         <v>15950</v>
@@ -1949,16 +1949,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.01613104921568008</v>
+        <v>0.01512274081242303</v>
       </c>
       <c r="C2" t="n">
         <v>0.04525804779853988</v>
       </c>
       <c r="D2" t="n">
-        <v>0.004257629970652742</v>
+        <v>0.004043673032953418</v>
       </c>
       <c r="E2" t="n">
-        <v>0.02269748542388596</v>
+        <v>0.02295223734114445</v>
       </c>
       <c r="F2" t="n">
         <v>0.1216971652958431</v>
@@ -1981,16 +1981,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.008113247404463496</v>
+        <v>0.007606110179460675</v>
       </c>
       <c r="C3" t="n">
         <v>0.01572121660370333</v>
       </c>
       <c r="D3" t="n">
-        <v>0.004276690339803879</v>
+        <v>0.004061775569168601</v>
       </c>
       <c r="E3" t="n">
-        <v>0.02276442158681893</v>
+        <v>0.02301992478183012</v>
       </c>
       <c r="F3" t="n">
         <v>0.1092790872044305</v>
@@ -2013,16 +2013,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.01017398126197526</v>
+        <v>0.01200344868318235</v>
       </c>
       <c r="C4" t="n">
         <v>0.02655138804181006</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00488946427680599</v>
+        <v>0.005387154237815462</v>
       </c>
       <c r="E4" t="n">
-        <v>0.02390778269961446</v>
+        <v>0.02542144699929226</v>
       </c>
       <c r="F4" t="n">
         <v>0.01600799782665798</v>
@@ -2045,16 +2045,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.05390735592077089</v>
+        <v>0.05053775241603135</v>
       </c>
       <c r="C5" t="n">
         <v>0.0003738669926515403</v>
       </c>
       <c r="D5" t="n">
-        <v>5.951661672896826e-06</v>
+        <v>5.652575252862016e-06</v>
       </c>
       <c r="E5" t="n">
-        <v>0.03779387872874857</v>
+        <v>0.03821806946560664</v>
       </c>
       <c r="F5" t="n">
         <v>0.09648063554985757</v>
@@ -2077,16 +2077,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.01015011986366353</v>
+        <v>0.01492755105678861</v>
       </c>
       <c r="C6" t="n">
         <v>0.08534374727724663</v>
       </c>
       <c r="D6" t="n">
-        <v>0.004880024815268958</v>
+        <v>0.006263662643034885</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02387803703935247</v>
+        <v>0.02660799243184001</v>
       </c>
       <c r="F6" t="n">
         <v>0.008636573020995315</v>
@@ -2109,16 +2109,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.05596808977828265</v>
+        <v>0.05493509091975302</v>
       </c>
       <c r="C7" t="n">
         <v>0.0003775290866890907</v>
       </c>
       <c r="D7" t="n">
-        <v>6.19750494683243e-06</v>
+        <v>6.185416146593732e-06</v>
       </c>
       <c r="E7" t="n">
-        <v>0.03773079161880303</v>
+        <v>0.03809747733592668</v>
       </c>
       <c r="F7" t="n">
         <v>0.0157028600381733</v>
@@ -2141,16 +2141,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.08442880779887192</v>
+        <v>0.07915139061153695</v>
       </c>
       <c r="C8" t="n">
         <v>0.0002269247205112488</v>
       </c>
       <c r="D8" t="n">
-        <v>5.271808030517261e-06</v>
+        <v>5.006886017537524e-06</v>
       </c>
       <c r="E8" t="n">
-        <v>0.04291232323088175</v>
+        <v>0.04339396233816271</v>
       </c>
       <c r="F8" t="n">
         <v>0.08636573020995315</v>
@@ -2173,16 +2173,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.006165080356366966</v>
+        <v>0.008245133366701168</v>
       </c>
       <c r="C9" t="n">
         <v>0.01711765704701222</v>
       </c>
       <c r="D9" t="n">
-        <v>0.005538165334464421</v>
+        <v>0.006739666653612321</v>
       </c>
       <c r="E9" t="n">
-        <v>0.02498348914255456</v>
+        <v>0.02721138937451249</v>
       </c>
       <c r="F9" t="n">
         <v>0.01588924413358189</v>
@@ -2205,16 +2205,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0498984550151626</v>
+        <v>0.04677943709955017</v>
       </c>
       <c r="C10" t="n">
         <v>0.0003709880765183546</v>
       </c>
       <c r="D10" t="n">
-        <v>5.110820785488384e-06</v>
+        <v>4.853988798695153e-06</v>
       </c>
       <c r="E10" t="n">
-        <v>0.04481705658614633</v>
+        <v>0.04532007402961995</v>
       </c>
       <c r="F10" t="n">
         <v>0.09232198746581198</v>
@@ -2237,16 +2237,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.006141218958055237</v>
+        <v>0.01116923574030743</v>
       </c>
       <c r="C11" t="n">
         <v>0.03079413561550136</v>
       </c>
       <c r="D11" t="n">
-        <v>0.005519481304246791</v>
+        <v>0.008478677509239843</v>
       </c>
       <c r="E11" t="n">
-        <v>0.02493027515935175</v>
+        <v>0.02881084924443909</v>
       </c>
       <c r="F11" t="n">
         <v>0.008601887988782482</v>
@@ -2269,16 +2269,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.05195918887267436</v>
+        <v>0.05117677560327184</v>
       </c>
       <c r="C12" t="n">
         <v>0.0003745937167451071</v>
       </c>
       <c r="D12" t="n">
-        <v>5.356713294631505e-06</v>
+        <v>5.386936448215256e-06</v>
       </c>
       <c r="E12" t="n">
-        <v>0.04418533685205702</v>
+        <v>0.04401841069799114</v>
       </c>
       <c r="F12" t="n">
         <v>0.01558857430281542</v>
@@ -2301,16 +2301,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.08041990689326363</v>
+        <v>0.07539307529505576</v>
       </c>
       <c r="C13" t="n">
         <v>0.0002258608842959221</v>
       </c>
       <c r="D13" t="n">
-        <v>4.767182317828934e-06</v>
+        <v>4.527619054415351e-06</v>
       </c>
       <c r="E13" t="n">
-        <v>0.04984292170031142</v>
+        <v>0.05040234842216126</v>
       </c>
       <c r="F13" t="n">
         <v>0.08301822128708675</v>
@@ -2333,16 +2333,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.05193532747436263</v>
+        <v>0.0541008779768781</v>
       </c>
       <c r="C14" t="n">
         <v>0.000378270131402864</v>
       </c>
       <c r="D14" t="n">
-        <v>5.352708887236377e-06</v>
+        <v>5.740966499468505e-06</v>
       </c>
       <c r="E14" t="n">
-        <v>0.04417298498619478</v>
+        <v>0.04335567385030175</v>
       </c>
       <c r="F14" t="n">
         <v>0.008512997254399197</v>
@@ -2365,16 +2365,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.08248064075077539</v>
+        <v>0.07979041379877744</v>
       </c>
       <c r="C15" t="n">
         <v>0.0002271922472913544</v>
       </c>
       <c r="D15" t="n">
-        <v>4.914729686443151e-06</v>
+        <v>4.847413451221902e-06</v>
       </c>
       <c r="E15" t="n">
-        <v>0.049075346950526</v>
+        <v>0.04877508126484811</v>
       </c>
       <c r="F15" t="n">
         <v>0.01529907220862027</v>
@@ -2397,16 +2397,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>9.544559324691378e-05</v>
+        <v>8.947954649831365e-05</v>
       </c>
       <c r="C16" t="n">
         <v>0.009512838072304559</v>
       </c>
       <c r="D16" t="n">
-        <v>0.07884499945653226</v>
+        <v>0.07488283394358181</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0603857851589331</v>
+        <v>0.06106354281609668</v>
       </c>
       <c r="F16" t="n">
         <v>0.09916065320402027</v>
@@ -2429,16 +2429,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.002132318052446946</v>
+        <v>0.007410920423826244</v>
       </c>
       <c r="C17" t="n">
         <v>0.01878635946354485</v>
       </c>
       <c r="D17" t="n">
-        <v>0.4133388665759593</v>
+        <v>0.4357284991145118</v>
       </c>
       <c r="E17" t="n">
-        <v>0.03731009896544584</v>
+        <v>0.0373952052171247</v>
       </c>
       <c r="F17" t="n">
         <v>0.008567480436827353</v>
@@ -2461,16 +2461,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.04795028796706607</v>
+        <v>0.04741846028679066</v>
       </c>
       <c r="C18" t="n">
         <v>0.0003717036408965787</v>
       </c>
       <c r="D18" t="n">
-        <v>4.515587516470138e-06</v>
+        <v>4.58813943862233e-06</v>
       </c>
       <c r="E18" t="n">
-        <v>0.06027704697807237</v>
+        <v>0.05748488084646997</v>
       </c>
       <c r="F18" t="n">
         <v>0.01547594009542513</v>
@@ -2493,16 +2493,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.07641100598765535</v>
+        <v>0.07163475997857459</v>
       </c>
       <c r="C19" t="n">
         <v>0.000224806976188473</v>
       </c>
       <c r="D19" t="n">
-        <v>4.262436283789588e-06</v>
+        <v>4.048237816401805e-06</v>
       </c>
       <c r="E19" t="n">
-        <v>0.06396874230026574</v>
+        <v>0.06468671433290586</v>
       </c>
       <c r="F19" t="n">
         <v>0.07992052646294172</v>
@@ -2525,16 +2525,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.04792642656875435</v>
+        <v>0.05034256266039692</v>
       </c>
       <c r="C20" t="n">
         <v>0.0003753232715591972</v>
       </c>
       <c r="D20" t="n">
-        <v>4.511582270679494e-06</v>
+        <v>4.942240423239806e-06</v>
       </c>
       <c r="E20" t="n">
-        <v>0.06027690209633611</v>
+        <v>0.05446732071311675</v>
       </c>
       <c r="F20" t="n">
         <v>0.008479295760913849</v>
@@ -2557,16 +2557,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.07847173984516712</v>
+        <v>0.07603209848229626</v>
       </c>
       <c r="C21" t="n">
         <v>0.0002261259071289186</v>
       </c>
       <c r="D21" t="n">
-        <v>4.410001385609817e-06</v>
+        <v>4.368070663818072e-06</v>
       </c>
       <c r="E21" t="n">
-        <v>0.06162709477936631</v>
+        <v>0.05985487191177444</v>
       </c>
       <c r="F21" t="n">
         <v>0.01519056815040311</v>
@@ -2589,16 +2589,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.002084595255823489</v>
+        <v>0.01473236130115418</v>
       </c>
       <c r="C22" t="n">
         <v>0.746757788675908</v>
       </c>
       <c r="D22" t="n">
-        <v>0.4783853899609822</v>
+        <v>0.4543452846015076</v>
       </c>
       <c r="E22" t="n">
-        <v>0.03685866761561508</v>
+        <v>0.03727236173491121</v>
       </c>
       <c r="F22" t="n">
         <v>0.004477153238308608</v>
@@ -2621,16 +2621,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.07844787844685537</v>
+        <v>0.07895620085590252</v>
       </c>
       <c r="C23" t="n">
         <v>0.0002274604056029539</v>
       </c>
       <c r="D23" t="n">
-        <v>4.407598234292715e-06</v>
+        <v>4.580531530054096e-06</v>
       </c>
       <c r="E23" t="n">
-        <v>0.06162814579067088</v>
+        <v>0.05747673365531459</v>
       </c>
       <c r="F23" t="n">
         <v>0.008392907951437453</v>
@@ -2653,16 +2653,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.09860783271861556</v>
+        <v>0.09244412290484241</v>
       </c>
       <c r="C24" t="n">
         <v>0.0001761753469474295</v>
       </c>
       <c r="D24" t="n">
-        <v>4.257629970652742e-06</v>
+        <v>4.043673032953418e-06</v>
       </c>
       <c r="E24" t="n">
-        <v>0.06397538461004745</v>
+        <v>0.06469343119460909</v>
       </c>
       <c r="F24" t="n">
         <v>0.06693344091271369</v>
@@ -2709,7 +2709,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.2771882676036963</v>
       </c>
     </row>
     <row r="3">
@@ -2717,7 +2717,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.07956211810363849</v>
       </c>
     </row>
     <row r="4">
@@ -2725,7 +2725,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.07596432089007199</v>
       </c>
     </row>
     <row r="5">
@@ -2733,7 +2733,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.0887594780761196</v>
       </c>
     </row>
     <row r="6">
@@ -2741,7 +2741,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.02904115627477501</v>
       </c>
     </row>
     <row r="7">
@@ -2749,7 +2749,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.03630892285481715</v>
       </c>
     </row>
     <row r="8">
@@ -2757,7 +2757,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.1080909842885875</v>
       </c>
     </row>
     <row r="9">
@@ -2765,7 +2765,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.05279605036889801</v>
       </c>
     </row>
     <row r="10">
@@ -2773,7 +2773,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.252288701539396</v>
       </c>
     </row>
   </sheetData>
@@ -2807,7 +2807,7 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1586222626906079</v>
+        <v>0.1240851971693286</v>
       </c>
     </row>
     <row r="3">
@@ -2815,7 +2815,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="n">
-        <v>0.06783556929757241</v>
+        <v>0.05909586467733745</v>
       </c>
     </row>
     <row r="4">
@@ -2823,143 +2823,143 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>0.05594411925592701</v>
+        <v>0.05305810104732629</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>0.04930300463870221</v>
+        <v>0.04885343389373953</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B6" t="n">
-        <v>0.04893763648895198</v>
+        <v>0.0483336870525143</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>0.04573300333552847</v>
+        <v>0.04747779785223569</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>0.04498973276679945</v>
+        <v>0.04645421345764324</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" t="n">
-        <v>0.04026179961382692</v>
+        <v>0.04604120066266992</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0400587730142406</v>
+        <v>0.04524206408060186</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>0.03993330261909819</v>
+        <v>0.04033785525800364</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B12" t="n">
-        <v>0.03939066304823054</v>
+        <v>0.03995929507450195</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B13" t="n">
-        <v>0.03886775312516076</v>
+        <v>0.03915635796245084</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0378034782959355</v>
+        <v>0.03902585477222233</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B15" t="n">
-        <v>0.03296211451876218</v>
+        <v>0.03789172916338462</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0320555767135463</v>
+        <v>0.03711911656684169</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B17" t="n">
-        <v>0.03195441866600065</v>
+        <v>0.03698702234251269</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.03177779156157975</v>
+        <v>0.03680366320696893</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B19" t="n">
-        <v>0.03141703646343348</v>
+        <v>0.03542152758696333</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B20" t="n">
-        <v>0.03123076889278729</v>
+        <v>0.02989529345926219</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" t="n">
-        <v>0.03108706756564101</v>
+        <v>0.02904117403357469</v>
       </c>
     </row>
     <row r="22">
@@ -2967,15 +2967,15 @@
         <v>2</v>
       </c>
       <c r="B22" t="n">
-        <v>0.02437085171766673</v>
+        <v>0.02806177221136825</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B23" t="n">
-        <v>0.02389227605020171</v>
+        <v>0.02646580541858433</v>
       </c>
     </row>
     <row r="24">
@@ -2983,7 +2983,7 @@
         <v>7</v>
       </c>
       <c r="B24" t="n">
-        <v>0.02157099965979882</v>
+        <v>0.02519197304996366</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix (bug #2): Error indicador 1.4
</commit_message>
<xml_diff>
--- a/Repo/Articulo1/output/AHP.xlsx
+++ b/Repo/Articulo1/output/AHP.xlsx
@@ -470,7 +470,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>03/13/23</t>
+          <t>04/02/23</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -793,7 +793,7 @@
         <v>39.9477784</v>
       </c>
       <c r="L5" t="n">
-        <v>0.715368279423794</v>
+        <v>0.958603951173407</v>
       </c>
       <c r="M5" t="n">
         <v>121.8776121123448</v>
@@ -905,7 +905,7 @@
         <v>39.5602784</v>
       </c>
       <c r="L7" t="n">
-        <v>0.6537430848820482</v>
+        <v>0.8510959963766491</v>
       </c>
       <c r="M7" t="n">
         <v>122.2633983069356</v>
@@ -961,7 +961,7 @@
         <v>65.81546400000002</v>
       </c>
       <c r="L8" t="n">
-        <v>0.8076223462626713</v>
+        <v>1.131928037118369</v>
       </c>
       <c r="M8" t="n">
         <v>107.3404408132477</v>
@@ -1073,7 +1073,7 @@
         <v>40.2577784</v>
       </c>
       <c r="L10" t="n">
-        <v>0.8330618797555602</v>
+        <v>1.182560277804791</v>
       </c>
       <c r="M10" t="n">
         <v>102.7784518394114</v>
@@ -1185,7 +1185,7 @@
         <v>39.8702784</v>
       </c>
       <c r="L12" t="n">
-        <v>0.7506442802556406</v>
+        <v>1.023100414119094</v>
       </c>
       <c r="M12" t="n">
         <v>105.8177015515107</v>
@@ -1241,7 +1241,7 @@
         <v>66.12546400000001</v>
       </c>
       <c r="L13" t="n">
-        <v>0.8931124691265738</v>
+        <v>1.30738877741298</v>
       </c>
       <c r="M13" t="n">
         <v>92.41488128683751</v>
@@ -1297,7 +1297,7 @@
         <v>39.4827784</v>
       </c>
       <c r="L14" t="n">
-        <v>0.7043540549013443</v>
+        <v>0.9389909155463747</v>
       </c>
       <c r="M14" t="n">
         <v>107.4352358608177</v>
@@ -1353,7 +1353,7 @@
         <v>65.73796400000002</v>
       </c>
       <c r="L15" t="n">
-        <v>0.8341918991733863</v>
+        <v>1.184877940454469</v>
       </c>
       <c r="M15" t="n">
         <v>95.49808888516999</v>
@@ -1521,7 +1521,7 @@
         <v>40.1802784</v>
       </c>
       <c r="L18" t="n">
-        <v>0.8813317657511304</v>
+        <v>1.282366543874901</v>
       </c>
       <c r="M18" t="n">
         <v>81.02873272804024</v>
@@ -1577,7 +1577,7 @@
         <v>66.43546400000001</v>
       </c>
       <c r="L19" t="n">
-        <v>0.9988724023500071</v>
+        <v>1.547292573912818</v>
       </c>
       <c r="M19" t="n">
         <v>72.00747624991654</v>
@@ -1633,7 +1633,7 @@
         <v>39.7927784</v>
       </c>
       <c r="L20" t="n">
-        <v>0.8181862245994608</v>
+        <v>1.152900358308349</v>
       </c>
       <c r="M20" t="n">
         <v>85.51782949900341</v>
@@ -1689,7 +1689,7 @@
         <v>66.04796400000001</v>
       </c>
       <c r="L21" t="n">
-        <v>0.9257343445581757</v>
+        <v>1.378578159221931</v>
       </c>
       <c r="M21" t="n">
         <v>77.82034940911073</v>
@@ -1801,7 +1801,7 @@
         <v>65.66046400000002</v>
       </c>
       <c r="L23" t="n">
-        <v>0.8827955896432095</v>
+        <v>1.28546803852881</v>
       </c>
       <c r="M23" t="n">
         <v>81.04021835940149</v>
@@ -1857,7 +1857,7 @@
         <v>84.77437980000001</v>
       </c>
       <c r="L24" t="n">
-        <v>1</v>
+        <v>1.55</v>
       </c>
       <c r="M24" t="n">
         <v>72</v>
@@ -1955,7 +1955,7 @@
         <v>0.04525804779853988</v>
       </c>
       <c r="D2" t="n">
-        <v>0.004043673032953418</v>
+        <v>0.00404375425268384</v>
       </c>
       <c r="E2" t="n">
         <v>0.02295223734114445</v>
@@ -1987,7 +1987,7 @@
         <v>0.01572121660370333</v>
       </c>
       <c r="D3" t="n">
-        <v>0.004061775569168601</v>
+        <v>0.004061857152499912</v>
       </c>
       <c r="E3" t="n">
         <v>0.02301992478183012</v>
@@ -2019,7 +2019,7 @@
         <v>0.02655138804181006</v>
       </c>
       <c r="D4" t="n">
-        <v>0.005387154237815462</v>
+        <v>0.005387262442215612</v>
       </c>
       <c r="E4" t="n">
         <v>0.02542144699929226</v>
@@ -2051,7 +2051,7 @@
         <v>0.0003738669926515403</v>
       </c>
       <c r="D5" t="n">
-        <v>5.652575252862016e-06</v>
+        <v>4.218378453097304e-06</v>
       </c>
       <c r="E5" t="n">
         <v>0.03821806946560664</v>
@@ -2083,7 +2083,7 @@
         <v>0.08534374727724663</v>
       </c>
       <c r="D6" t="n">
-        <v>0.006263662643034885</v>
+        <v>0.00626378845266073</v>
       </c>
       <c r="E6" t="n">
         <v>0.02660799243184001</v>
@@ -2115,7 +2115,7 @@
         <v>0.0003775290866890907</v>
       </c>
       <c r="D7" t="n">
-        <v>6.185416146593732e-06</v>
+        <v>4.751231670574434e-06</v>
       </c>
       <c r="E7" t="n">
         <v>0.03809747733592668</v>
@@ -2147,7 +2147,7 @@
         <v>0.0002269247205112488</v>
       </c>
       <c r="D8" t="n">
-        <v>5.006886017537524e-06</v>
+        <v>3.572448176986866e-06</v>
       </c>
       <c r="E8" t="n">
         <v>0.04339396233816271</v>
@@ -2179,7 +2179,7 @@
         <v>0.01711765704701222</v>
       </c>
       <c r="D9" t="n">
-        <v>0.006739666653612321</v>
+        <v>0.006739802024079785</v>
       </c>
       <c r="E9" t="n">
         <v>0.02721138937451249</v>
@@ -2211,7 +2211,7 @@
         <v>0.0003709880765183546</v>
       </c>
       <c r="D10" t="n">
-        <v>4.853988798695153e-06</v>
+        <v>3.419491021794115e-06</v>
       </c>
       <c r="E10" t="n">
         <v>0.04532007402961995</v>
@@ -2243,7 +2243,7 @@
         <v>0.03079413561550136</v>
       </c>
       <c r="D11" t="n">
-        <v>0.008478677509239843</v>
+        <v>0.008478847808840237</v>
       </c>
       <c r="E11" t="n">
         <v>0.02881084924443909</v>
@@ -2275,7 +2275,7 @@
         <v>0.0003745937167451071</v>
       </c>
       <c r="D12" t="n">
-        <v>5.386936448215256e-06</v>
+        <v>3.952450997848124e-06</v>
       </c>
       <c r="E12" t="n">
         <v>0.04401841069799114</v>
@@ -2307,7 +2307,7 @@
         <v>0.0002258608842959221</v>
       </c>
       <c r="D13" t="n">
-        <v>4.527619054415351e-06</v>
+        <v>3.093000584482217e-06</v>
       </c>
       <c r="E13" t="n">
         <v>0.05040234842216126</v>
@@ -2339,7 +2339,7 @@
         <v>0.000378270131402864</v>
       </c>
       <c r="D14" t="n">
-        <v>5.740966499468505e-06</v>
+        <v>4.306489217023876e-06</v>
       </c>
       <c r="E14" t="n">
         <v>0.04335567385030175</v>
@@ -2371,7 +2371,7 @@
         <v>0.0002271922472913544</v>
       </c>
       <c r="D15" t="n">
-        <v>4.847413451221902e-06</v>
+        <v>3.412802377882761e-06</v>
       </c>
       <c r="E15" t="n">
         <v>0.04877508126484811</v>
@@ -2403,7 +2403,7 @@
         <v>0.009512838072304559</v>
       </c>
       <c r="D16" t="n">
-        <v>0.07488283394358181</v>
+        <v>0.0748843380126637</v>
       </c>
       <c r="E16" t="n">
         <v>0.06106354281609668</v>
@@ -2435,7 +2435,7 @@
         <v>0.01878635946354485</v>
       </c>
       <c r="D17" t="n">
-        <v>0.4357284991145118</v>
+        <v>0.4357372509970074</v>
       </c>
       <c r="E17" t="n">
         <v>0.0373952052171247</v>
@@ -2467,7 +2467,7 @@
         <v>0.0003717036408965787</v>
       </c>
       <c r="D18" t="n">
-        <v>4.58813943862233e-06</v>
+        <v>3.153352894301896e-06</v>
       </c>
       <c r="E18" t="n">
         <v>0.05748488084646997</v>
@@ -2499,7 +2499,7 @@
         <v>0.000224806976188473</v>
       </c>
       <c r="D19" t="n">
-        <v>4.048237816401805e-06</v>
+        <v>2.6134386740175e-06</v>
       </c>
       <c r="E19" t="n">
         <v>0.06468671433290586</v>
@@ -2531,7 +2531,7 @@
         <v>0.0003753232715591972</v>
       </c>
       <c r="D20" t="n">
-        <v>4.942240423239806e-06</v>
+        <v>3.507462048686707e-06</v>
       </c>
       <c r="E20" t="n">
         <v>0.05446732071311675</v>
@@ -2563,7 +2563,7 @@
         <v>0.0002261259071289186</v>
       </c>
       <c r="D21" t="n">
-        <v>4.368070663818072e-06</v>
+        <v>2.933278919032153e-06</v>
       </c>
       <c r="E21" t="n">
         <v>0.05985487191177444</v>
@@ -2595,7 +2595,7 @@
         <v>0.746757788675908</v>
       </c>
       <c r="D22" t="n">
-        <v>0.4543452846015076</v>
+        <v>0.4543544104139146</v>
       </c>
       <c r="E22" t="n">
         <v>0.03727236173491121</v>
@@ -2627,7 +2627,7 @@
         <v>0.0002274604056029539</v>
       </c>
       <c r="D23" t="n">
-        <v>4.580531530054096e-06</v>
+        <v>3.145744687134988e-06</v>
       </c>
       <c r="E23" t="n">
         <v>0.05747673365531459</v>
@@ -2659,7 +2659,7 @@
         <v>0.0001761753469474295</v>
       </c>
       <c r="D24" t="n">
-        <v>4.043673032953418e-06</v>
+        <v>2.608873711408929e-06</v>
       </c>
       <c r="E24" t="n">
         <v>0.06469343119460909</v>
@@ -2807,7 +2807,7 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1240851971693286</v>
+        <v>0.1240858904054707</v>
       </c>
     </row>
     <row r="3">
@@ -2815,7 +2815,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="n">
-        <v>0.05909586467733745</v>
+        <v>0.05909652950814774</v>
       </c>
     </row>
     <row r="4">
@@ -2823,7 +2823,7 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>0.05305810104732629</v>
+        <v>0.05305799205377021</v>
       </c>
     </row>
     <row r="5">
@@ -2831,7 +2831,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>0.04885343389373953</v>
+        <v>0.0488533249276431</v>
       </c>
     </row>
     <row r="6">
@@ -2839,7 +2839,7 @@
         <v>21</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0483336870525143</v>
+        <v>0.04833357805990615</v>
       </c>
     </row>
     <row r="7">
@@ -2847,7 +2847,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>0.04747779785223569</v>
+        <v>0.04747768887297976</v>
       </c>
     </row>
     <row r="8">
@@ -2855,7 +2855,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="n">
-        <v>0.04645421345764324</v>
+        <v>0.04645410447782543</v>
       </c>
     </row>
     <row r="9">
@@ -2863,7 +2863,7 @@
         <v>19</v>
       </c>
       <c r="B9" t="n">
-        <v>0.04604120066266992</v>
+        <v>0.04604109166968942</v>
       </c>
     </row>
     <row r="10">
@@ -2871,7 +2871,7 @@
         <v>17</v>
       </c>
       <c r="B10" t="n">
-        <v>0.04524206408060186</v>
+        <v>0.0452419550870594</v>
       </c>
     </row>
     <row r="11">
@@ -2879,7 +2879,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>0.04033785525800364</v>
+        <v>0.04033774628891104</v>
       </c>
     </row>
     <row r="12">
@@ -2887,7 +2887,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="n">
-        <v>0.03995929507450195</v>
+        <v>0.03995918612765219</v>
       </c>
     </row>
     <row r="13">
@@ -2895,7 +2895,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="n">
-        <v>0.03915635796245084</v>
+        <v>0.03915624901466493</v>
       </c>
     </row>
     <row r="14">
@@ -2903,7 +2903,7 @@
         <v>18</v>
       </c>
       <c r="B14" t="n">
-        <v>0.03902585477222233</v>
+        <v>0.03902574578025748</v>
       </c>
     </row>
     <row r="15">
@@ -2911,7 +2911,7 @@
         <v>10</v>
       </c>
       <c r="B15" t="n">
-        <v>0.03789172916338462</v>
+        <v>0.03789162019367157</v>
       </c>
     </row>
     <row r="16">
@@ -2919,7 +2919,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="n">
-        <v>0.03711911656684169</v>
+        <v>0.03711900759619224</v>
       </c>
     </row>
     <row r="17">
@@ -2927,7 +2927,7 @@
         <v>0</v>
       </c>
       <c r="B17" t="n">
-        <v>0.03698702234251269</v>
+        <v>0.03698702851231435</v>
       </c>
     </row>
     <row r="18">
@@ -2935,7 +2935,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.03680366320696893</v>
+        <v>0.03680355421438346</v>
       </c>
     </row>
     <row r="19">
@@ -2943,7 +2943,7 @@
         <v>4</v>
       </c>
       <c r="B19" t="n">
-        <v>0.03542152758696333</v>
+        <v>0.03542153714400613</v>
       </c>
     </row>
     <row r="20">
@@ -2951,7 +2951,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="n">
-        <v>0.02989529345926219</v>
+        <v>0.02989540771484856</v>
       </c>
     </row>
     <row r="21">
@@ -2959,7 +2959,7 @@
         <v>9</v>
       </c>
       <c r="B21" t="n">
-        <v>0.02904117403357469</v>
+        <v>0.02904118697026819</v>
       </c>
     </row>
     <row r="22">
@@ -2967,7 +2967,7 @@
         <v>2</v>
       </c>
       <c r="B22" t="n">
-        <v>0.02806177221136825</v>
+        <v>0.02806178043104202</v>
       </c>
     </row>
     <row r="23">
@@ -2975,7 +2975,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="n">
-        <v>0.02646580541858433</v>
+        <v>0.02646581161600669</v>
       </c>
     </row>
     <row r="24">
@@ -2983,7 +2983,7 @@
         <v>7</v>
       </c>
       <c r="B24" t="n">
-        <v>0.02519197304996366</v>
+        <v>0.02519198333328929</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: visualización de graficas recurso hidrico
</commit_message>
<xml_diff>
--- a/Repo/Articulo1/output/AHP.xlsx
+++ b/Repo/Articulo1/output/AHP.xlsx
@@ -470,7 +470,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>04/02/23</t>
+          <t>07/11/23</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -722,7 +722,7 @@
         <v>1918.506818181818</v>
       </c>
       <c r="G4" t="n">
-        <v>640.793947259624</v>
+        <v>640.7939472596241</v>
       </c>
       <c r="H4" t="n">
         <v>4.540635118306349</v>
@@ -849,10 +849,10 @@
         <v>0.175</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0006455764403994414</v>
+        <v>0.0006455764403994413</v>
       </c>
       <c r="M6" t="n">
-        <v>175.0574402764045</v>
+        <v>175.0574402764044</v>
       </c>
       <c r="N6" t="n">
         <v>15500</v>
@@ -890,7 +890,7 @@
         <v>1918.506818181818</v>
       </c>
       <c r="G7" t="n">
-        <v>640.793947259624</v>
+        <v>640.7939472596241</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1002,7 +1002,7 @@
         <v>959.2534090909091</v>
       </c>
       <c r="G9" t="n">
-        <v>640.793947259624</v>
+        <v>640.7939472596241</v>
       </c>
       <c r="H9" t="n">
         <v>9.081270236612697</v>
@@ -1170,7 +1170,7 @@
         <v>959.2534090909091</v>
       </c>
       <c r="G12" t="n">
-        <v>640.793947259624</v>
+        <v>640.7939472596241</v>
       </c>
       <c r="H12" t="n">
         <v>4.540635118306349</v>
@@ -1338,7 +1338,7 @@
         <v>959.2534090909091</v>
       </c>
       <c r="G15" t="n">
-        <v>640.793947259624</v>
+        <v>640.7939472596241</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1506,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>640.793947259624</v>
+        <v>640.7939472596241</v>
       </c>
       <c r="H18" t="n">
         <v>9.081270236612697</v>
@@ -1674,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>640.793947259624</v>
+        <v>640.7939472596241</v>
       </c>
       <c r="H21" t="n">
         <v>4.540635118306349</v>
@@ -1730,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>2135.979824198747</v>
+        <v>2135.979824198748</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -1804,7 +1804,7 @@
         <v>1.28546803852881</v>
       </c>
       <c r="M23" t="n">
-        <v>81.04021835940149</v>
+        <v>81.04021835940151</v>
       </c>
       <c r="N23" t="n">
         <v>15950</v>
@@ -2083,10 +2083,10 @@
         <v>0.08534374727724663</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00626378845266073</v>
+        <v>0.006263788452660731</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02660799243184001</v>
+        <v>0.02660799243184002</v>
       </c>
       <c r="F6" t="n">
         <v>0.008636573020995315</v>
@@ -2429,7 +2429,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.007410920423826244</v>
+        <v>0.007410920423826245</v>
       </c>
       <c r="C17" t="n">
         <v>0.01878635946354485</v>
@@ -2531,7 +2531,7 @@
         <v>0.0003753232715591972</v>
       </c>
       <c r="D20" t="n">
-        <v>3.507462048686707e-06</v>
+        <v>3.507462048686708e-06</v>
       </c>
       <c r="E20" t="n">
         <v>0.05446732071311675</v>
@@ -2630,7 +2630,7 @@
         <v>3.145744687134988e-06</v>
       </c>
       <c r="E23" t="n">
-        <v>0.05747673365531459</v>
+        <v>0.05747673365531458</v>
       </c>
       <c r="F23" t="n">
         <v>0.008392907951437453</v>

</xml_diff>

<commit_message>
fix: contrucción grafico de resultados
</commit_message>
<xml_diff>
--- a/Repo/Articulo1/output/AHP.xlsx
+++ b/Repo/Articulo1/output/AHP.xlsx
@@ -470,7 +470,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>07/11/23</t>
+          <t>07/17/23</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -722,7 +722,7 @@
         <v>1918.506818181818</v>
       </c>
       <c r="G4" t="n">
-        <v>640.7939472596241</v>
+        <v>640.793947259624</v>
       </c>
       <c r="H4" t="n">
         <v>4.540635118306349</v>
@@ -849,10 +849,10 @@
         <v>0.175</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0006455764403994413</v>
+        <v>0.0006455764403994414</v>
       </c>
       <c r="M6" t="n">
-        <v>175.0574402764044</v>
+        <v>175.0574402764045</v>
       </c>
       <c r="N6" t="n">
         <v>15500</v>
@@ -890,7 +890,7 @@
         <v>1918.506818181818</v>
       </c>
       <c r="G7" t="n">
-        <v>640.7939472596241</v>
+        <v>640.793947259624</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -1002,7 +1002,7 @@
         <v>959.2534090909091</v>
       </c>
       <c r="G9" t="n">
-        <v>640.7939472596241</v>
+        <v>640.793947259624</v>
       </c>
       <c r="H9" t="n">
         <v>9.081270236612697</v>
@@ -1170,7 +1170,7 @@
         <v>959.2534090909091</v>
       </c>
       <c r="G12" t="n">
-        <v>640.7939472596241</v>
+        <v>640.793947259624</v>
       </c>
       <c r="H12" t="n">
         <v>4.540635118306349</v>
@@ -1338,7 +1338,7 @@
         <v>959.2534090909091</v>
       </c>
       <c r="G15" t="n">
-        <v>640.7939472596241</v>
+        <v>640.793947259624</v>
       </c>
       <c r="H15" t="n">
         <v>0</v>
@@ -1506,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>640.7939472596241</v>
+        <v>640.793947259624</v>
       </c>
       <c r="H18" t="n">
         <v>9.081270236612697</v>
@@ -1674,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>640.7939472596241</v>
+        <v>640.793947259624</v>
       </c>
       <c r="H21" t="n">
         <v>4.540635118306349</v>
@@ -1730,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>2135.979824198748</v>
+        <v>2135.979824198747</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -1804,7 +1804,7 @@
         <v>1.28546803852881</v>
       </c>
       <c r="M23" t="n">
-        <v>81.04021835940151</v>
+        <v>81.04021835940149</v>
       </c>
       <c r="N23" t="n">
         <v>15950</v>
@@ -2083,10 +2083,10 @@
         <v>0.08534374727724663</v>
       </c>
       <c r="D6" t="n">
-        <v>0.006263788452660731</v>
+        <v>0.00626378845266073</v>
       </c>
       <c r="E6" t="n">
-        <v>0.02660799243184002</v>
+        <v>0.02660799243184001</v>
       </c>
       <c r="F6" t="n">
         <v>0.008636573020995315</v>
@@ -2429,7 +2429,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.007410920423826245</v>
+        <v>0.007410920423826244</v>
       </c>
       <c r="C17" t="n">
         <v>0.01878635946354485</v>
@@ -2531,7 +2531,7 @@
         <v>0.0003753232715591972</v>
       </c>
       <c r="D20" t="n">
-        <v>3.507462048686708e-06</v>
+        <v>3.507462048686707e-06</v>
       </c>
       <c r="E20" t="n">
         <v>0.05446732071311675</v>
@@ -2630,7 +2630,7 @@
         <v>3.145744687134988e-06</v>
       </c>
       <c r="E23" t="n">
-        <v>0.05747673365531458</v>
+        <v>0.05747673365531459</v>
       </c>
       <c r="F23" t="n">
         <v>0.008392907951437453</v>

</xml_diff>